<commit_message>
updating spreadsheet with better variable names
</commit_message>
<xml_diff>
--- a/Olive Oil Experiment Participant List_2_25_22.xlsx
+++ b/Olive Oil Experiment Participant List_2_25_22.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hannahgross/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hannahgross/Desktop/W241/Final Project/Olive_Oil_Taste_Test/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB713EE1-B0B4-FD43-B454-235DD68957DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95E66317-E177-B841-B4C8-E27FF44389B7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16280" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="171" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="182" uniqueCount="75">
   <si>
     <t>Pre-Test</t>
   </si>
@@ -235,13 +235,46 @@
   </si>
   <si>
     <t xml:space="preserve">Katharine </t>
+  </si>
+  <si>
+    <t>admin</t>
+  </si>
+  <si>
+    <t>name</t>
+  </si>
+  <si>
+    <t>age</t>
+  </si>
+  <si>
+    <t>tasting_count</t>
+  </si>
+  <si>
+    <t>birth_country</t>
+  </si>
+  <si>
+    <t>covid</t>
+  </si>
+  <si>
+    <t>azzignment</t>
+  </si>
+  <si>
+    <t>first_oo</t>
+  </si>
+  <si>
+    <t>smell_outcome</t>
+  </si>
+  <si>
+    <t>bitter_outcome</t>
+  </si>
+  <si>
+    <t>better_oo</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -257,6 +290,12 @@
       <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -279,13 +318,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -293,6 +333,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -511,10 +552,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:K39"/>
+  <dimension ref="A1:AB40"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G17" sqref="G17"/>
+      <selection activeCell="G23" sqref="G23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -527,26 +568,26 @@
     <col min="7" max="7" width="23.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="1"/>
       <c r="B1" s="1"/>
-      <c r="C1" s="4" t="s">
+      <c r="C1" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="5"/>
-      <c r="E1" s="5"/>
-      <c r="F1" s="5"/>
-      <c r="G1" s="6" t="s">
+      <c r="D1" s="6"/>
+      <c r="E1" s="6"/>
+      <c r="F1" s="6"/>
+      <c r="G1" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="H1" s="5"/>
-      <c r="I1" s="6" t="s">
+      <c r="H1" s="6"/>
+      <c r="I1" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="J1" s="5"/>
-      <c r="K1" s="5"/>
-    </row>
-    <row r="2" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="J1" s="6"/>
+      <c r="K1" s="6"/>
+    </row>
+    <row r="2" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="1" t="s">
         <v>3</v>
       </c>
@@ -581,55 +622,87 @@
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A3" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="B3" s="3" t="s">
+    <row r="3" spans="1:28" s="4" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A3" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="B3" s="8" t="s">
+        <v>65</v>
+      </c>
+      <c r="C3" s="8" t="s">
+        <v>66</v>
+      </c>
+      <c r="D3" s="8" t="s">
+        <v>67</v>
+      </c>
+      <c r="E3" s="8" t="s">
+        <v>68</v>
+      </c>
+      <c r="F3" s="8" t="s">
+        <v>69</v>
+      </c>
+      <c r="G3" s="8" t="s">
+        <v>70</v>
+      </c>
+      <c r="H3" s="8" t="s">
+        <v>71</v>
+      </c>
+      <c r="I3" s="8" t="s">
+        <v>72</v>
+      </c>
+      <c r="J3" s="8" t="s">
+        <v>73</v>
+      </c>
+      <c r="K3" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="L3" s="8"/>
+      <c r="M3" s="8"/>
+      <c r="N3" s="8"/>
+      <c r="O3" s="8"/>
+      <c r="P3" s="8"/>
+      <c r="Q3" s="8"/>
+      <c r="R3" s="8"/>
+      <c r="S3" s="8"/>
+      <c r="T3" s="8"/>
+      <c r="U3" s="8"/>
+      <c r="V3" s="8"/>
+      <c r="W3" s="8"/>
+      <c r="X3" s="8"/>
+      <c r="Y3" s="8"/>
+      <c r="Z3" s="8"/>
+      <c r="AA3" s="8"/>
+      <c r="AB3" s="8"/>
+    </row>
+    <row r="4" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A4" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B4" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="C3" s="3">
+      <c r="C4" s="3">
         <v>33</v>
       </c>
-      <c r="D3" s="3" t="s">
+      <c r="D4" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="E3" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="F3" s="3" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A4" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="B4" s="3" t="s">
+      <c r="E4" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="5" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A5" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B5" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="C4" s="3">
+      <c r="C5" s="3">
         <v>65</v>
-      </c>
-      <c r="D4" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="E4" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="F4" s="3" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A5" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="B5" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="C5" s="3">
-        <v>64</v>
       </c>
       <c r="D5" s="3" t="s">
         <v>20</v>
@@ -641,15 +714,15 @@
         <v>18</v>
       </c>
     </row>
-    <row r="6" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" s="3" t="s">
         <v>14</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C6" s="3">
-        <v>25</v>
+        <v>64</v>
       </c>
       <c r="D6" s="3" t="s">
         <v>20</v>
@@ -661,15 +734,15 @@
         <v>18</v>
       </c>
     </row>
-    <row r="7" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" s="3" t="s">
         <v>14</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C7" s="3">
-        <v>55</v>
+        <v>25</v>
       </c>
       <c r="D7" s="3" t="s">
         <v>20</v>
@@ -681,15 +754,15 @@
         <v>18</v>
       </c>
     </row>
-    <row r="8" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" s="3" t="s">
         <v>14</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C8" s="3">
-        <v>38</v>
+        <v>55</v>
       </c>
       <c r="D8" s="3" t="s">
         <v>20</v>
@@ -698,21 +771,21 @@
         <v>17</v>
       </c>
       <c r="F8" s="3" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="9" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" s="3" t="s">
         <v>14</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C9" s="3">
         <v>38</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="E9" s="3" t="s">
         <v>17</v>
@@ -721,72 +794,72 @@
         <v>25</v>
       </c>
     </row>
-    <row r="10" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" s="3" t="s">
         <v>14</v>
       </c>
       <c r="B10" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="C10" s="3">
+        <v>38</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="E10" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="F10" s="3" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="11" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A11" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B11" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="C10" s="3">
+      <c r="C11" s="3">
         <v>34</v>
       </c>
-      <c r="D10" s="3" t="s">
+      <c r="D11" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="E10" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="F10" s="3" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="11" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A11" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="B11" s="3" t="s">
+      <c r="E11" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="F11" s="3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="12" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A12" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B12" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="C11" s="3">
+      <c r="C12" s="3">
         <v>33</v>
       </c>
-      <c r="D11" s="3" t="s">
+      <c r="D12" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="E11" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="F11" s="3" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="12" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A12" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="B12" s="3" t="s">
+      <c r="E12" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="F12" s="3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="13" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A13" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B13" s="3" t="s">
         <v>29</v>
-      </c>
-      <c r="C12" s="3">
-        <v>35</v>
-      </c>
-      <c r="D12" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="E12" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="F12" s="3" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="13" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A13" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="B13" s="3" t="s">
-        <v>30</v>
       </c>
       <c r="C13" s="3">
         <v>35</v>
@@ -801,15 +874,15 @@
         <v>18</v>
       </c>
     </row>
-    <row r="14" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A14" s="3" t="s">
         <v>14</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C14" s="3">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="D14" s="3" t="s">
         <v>20</v>
@@ -821,12 +894,12 @@
         <v>18</v>
       </c>
     </row>
-    <row r="15" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A15" s="3" t="s">
         <v>14</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C15" s="3">
         <v>33</v>
@@ -841,15 +914,15 @@
         <v>18</v>
       </c>
     </row>
-    <row r="16" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A16" s="3" t="s">
         <v>14</v>
       </c>
       <c r="B16" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="C16" s="3">
         <v>33</v>
-      </c>
-      <c r="C16" s="3">
-        <v>34</v>
       </c>
       <c r="D16" s="3" t="s">
         <v>20</v>
@@ -858,7 +931,7 @@
         <v>17</v>
       </c>
       <c r="F16" s="3" t="s">
-        <v>25</v>
+        <v>18</v>
       </c>
     </row>
     <row r="17" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -866,7 +939,7 @@
         <v>14</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C17" s="3">
         <v>34</v>
@@ -886,7 +959,7 @@
         <v>14</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C18" s="3">
         <v>34</v>
@@ -898,24 +971,24 @@
         <v>17</v>
       </c>
       <c r="F18" s="3" t="s">
-        <v>18</v>
+        <v>25</v>
       </c>
     </row>
     <row r="19" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A19" s="3" t="s">
-        <v>36</v>
+        <v>14</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C19" s="3">
-        <v>61</v>
+        <v>34</v>
       </c>
       <c r="D19" s="3" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="E19" s="3" t="s">
-        <v>38</v>
+        <v>17</v>
       </c>
       <c r="F19" s="3" t="s">
         <v>18</v>
@@ -926,13 +999,16 @@
         <v>36</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>39</v>
+        <v>37</v>
+      </c>
+      <c r="C20" s="3">
+        <v>61</v>
       </c>
       <c r="D20" s="3" t="s">
         <v>16</v>
       </c>
       <c r="E20" s="3" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="F20" s="3" t="s">
         <v>18</v>
@@ -943,16 +1019,13 @@
         <v>36</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="C21" s="3">
-        <v>22</v>
+        <v>39</v>
       </c>
       <c r="D21" s="3" t="s">
         <v>16</v>
       </c>
       <c r="E21" s="3" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="F21" s="3" t="s">
         <v>18</v>
@@ -963,13 +1036,13 @@
         <v>36</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C22" s="3">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="D22" s="3" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="E22" s="3" t="s">
         <v>42</v>
@@ -983,19 +1056,19 @@
         <v>36</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C23" s="3">
         <v>25</v>
       </c>
       <c r="D23" s="3" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="E23" s="3" t="s">
         <v>42</v>
       </c>
       <c r="F23" s="3" t="s">
-        <v>25</v>
+        <v>18</v>
       </c>
     </row>
     <row r="24" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -1003,19 +1076,19 @@
         <v>36</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C24" s="3">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="D24" s="3" t="s">
         <v>16</v>
       </c>
       <c r="E24" s="3" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="F24" s="3" t="s">
-        <v>18</v>
+        <v>25</v>
       </c>
     </row>
     <row r="25" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -1023,13 +1096,19 @@
         <v>36</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>47</v>
+        <v>45</v>
+      </c>
+      <c r="C25" s="3">
+        <v>28</v>
       </c>
       <c r="D25" s="3" t="s">
         <v>16</v>
       </c>
       <c r="E25" s="3" t="s">
-        <v>38</v>
+        <v>46</v>
+      </c>
+      <c r="F25" s="3" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="26" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -1037,13 +1116,13 @@
         <v>36</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D26" s="3" t="s">
         <v>16</v>
       </c>
       <c r="E26" s="3" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="27" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -1051,7 +1130,7 @@
         <v>36</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D27" s="3" t="s">
         <v>16</v>
@@ -1065,13 +1144,13 @@
         <v>36</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D28" s="3" t="s">
         <v>16</v>
       </c>
       <c r="E28" s="3" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="29" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -1079,7 +1158,10 @@
         <v>36</v>
       </c>
       <c r="B29" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
+      </c>
+      <c r="D29" s="3" t="s">
+        <v>16</v>
       </c>
       <c r="E29" s="3" t="s">
         <v>42</v>
@@ -1087,19 +1169,13 @@
     </row>
     <row r="30" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A30" s="3" t="s">
-        <v>52</v>
+        <v>36</v>
       </c>
       <c r="B30" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="C30" s="3">
-        <v>24</v>
+        <v>51</v>
       </c>
       <c r="E30" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="F30" s="3" t="s">
-        <v>25</v>
+        <v>42</v>
       </c>
     </row>
     <row r="31" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -1107,13 +1183,13 @@
         <v>52</v>
       </c>
       <c r="B31" s="3" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C31" s="3">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E31" s="3" t="s">
-        <v>42</v>
+        <v>54</v>
       </c>
       <c r="F31" s="3" t="s">
         <v>25</v>
@@ -1124,7 +1200,7 @@
         <v>52</v>
       </c>
       <c r="B32" s="3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C32" s="3">
         <v>25</v>
@@ -1133,68 +1209,85 @@
         <v>42</v>
       </c>
       <c r="F32" s="3" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="33" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A33" s="3" t="s">
-        <v>36</v>
+        <v>52</v>
       </c>
       <c r="B33" s="3" t="s">
-        <v>57</v>
+        <v>56</v>
+      </c>
+      <c r="C33" s="3">
+        <v>25</v>
       </c>
       <c r="E33" s="3" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="34" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="F33" s="3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A34" s="3" t="s">
         <v>36</v>
       </c>
       <c r="B34" s="3" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E34" s="3" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="35" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="35" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A35" s="3" t="s">
         <v>36</v>
       </c>
       <c r="B35" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="E35" s="3" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A36" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="B36" s="3" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="36" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A36" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="B36" s="3" t="s">
+    <row r="37" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A37" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="B37" s="3" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="37" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A37" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="B37" s="3" t="s">
+    <row r="38" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A38" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="B38" s="3" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="38" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A38" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="B38" s="3" t="s">
+    <row r="39" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A39" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="B39" s="3" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="39" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A39" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="B39" s="3" t="s">
+    <row r="40" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A40" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="B40" s="3" t="s">
         <v>63</v>
       </c>
     </row>

</xml_diff>